<commit_message>
Style changes, added assets, nav buttons
</commit_message>
<xml_diff>
--- a/coordinates.xlsx
+++ b/coordinates.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -447,8 +447,8 @@
         <v>-520</v>
       </c>
       <c r="D2" t="str">
-        <f xml:space="preserve"> "{ x:" &amp; B2 &amp; ", z:" &amp; C2 &amp; ", id: 'p" &amp; A2 &amp; "', imageUrl: 'assets/" &amp; A2 &amp; "', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },"</f>
-        <v>{ x:386, z:-520, id: 'p1', imageUrl: 'assets/1', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <f xml:space="preserve"> "{ x:" &amp; B2 &amp; ", z:" &amp; C2 &amp; ", id: 'p" &amp; A2 &amp; "', imageUrl: 'assets/" &amp; A2 &amp; "', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: " &amp; A2 -1 &amp;" },"</f>
+        <v>{ x:386, z:-520, id: 'p1', imageUrl: 'assets/1', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 0 },</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -463,8 +463,8 @@
         <v>-496</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D26" si="0" xml:space="preserve"> "{ x:" &amp; B3 &amp; ", z:" &amp; C3 &amp; ", id: 'p" &amp; A3 &amp; "', imageUrl: 'assets/" &amp; A3 &amp; "', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },"</f>
-        <v>{ x:433, z:-496, id: 'p2', imageUrl: 'assets/2', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <f t="shared" ref="D3:D26" si="0" xml:space="preserve"> "{ x:" &amp; B3 &amp; ", z:" &amp; C3 &amp; ", id: 'p" &amp; A3 &amp; "', imageUrl: 'assets/" &amp; A3 &amp; "', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: " &amp; A3 -1 &amp;" },"</f>
+        <v>{ x:433, z:-496, id: 'p2', imageUrl: 'assets/2', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 1 },</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -480,7 +480,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:260, z:-421, id: 'p3', imageUrl: 'assets/3', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:260, z:-421, id: 'p3', imageUrl: 'assets/3', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 2 },</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -496,7 +496,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:290, z:-375, id: 'p4', imageUrl: 'assets/4', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:290, z:-375, id: 'p4', imageUrl: 'assets/4', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 3 },</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -512,7 +512,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:133, z:-476, id: 'p5', imageUrl: 'assets/5', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:133, z:-476, id: 'p5', imageUrl: 'assets/5', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 4 },</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -528,7 +528,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:16, z:-543, id: 'p6', imageUrl: 'assets/6', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:16, z:-543, id: 'p6', imageUrl: 'assets/6', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 5 },</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -544,7 +544,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-80, z:-634, id: 'p7', imageUrl: 'assets/7', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-80, z:-634, id: 'p7', imageUrl: 'assets/7', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 6 },</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -560,7 +560,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-156, z:-831, id: 'p8', imageUrl: 'assets/8', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-156, z:-831, id: 'p8', imageUrl: 'assets/8', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 7 },</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -576,7 +576,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-90, z:-818, id: 'p9', imageUrl: 'assets/9', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-90, z:-818, id: 'p9', imageUrl: 'assets/9', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 8 },</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -592,7 +592,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-243, z:-868, id: 'p10', imageUrl: 'assets/10', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-243, z:-868, id: 'p10', imageUrl: 'assets/10', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 9 },</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -608,7 +608,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-203, z:-910, id: 'p11', imageUrl: 'assets/11', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-203, z:-910, id: 'p11', imageUrl: 'assets/11', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 10 },</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -624,7 +624,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-354, z:-970, id: 'p12', imageUrl: 'assets/12', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-354, z:-970, id: 'p12', imageUrl: 'assets/12', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 11 },</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -640,7 +640,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-783, z:-1248, id: 'p13', imageUrl: 'assets/13', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-783, z:-1248, id: 'p13', imageUrl: 'assets/13', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 12 },</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -656,7 +656,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-530, z:-1117, id: 'p14', imageUrl: 'assets/14', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-530, z:-1117, id: 'p14', imageUrl: 'assets/14', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 13 },</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -672,7 +672,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:-140, z:-593, id: 'p15', imageUrl: 'assets/15', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:-140, z:-593, id: 'p15', imageUrl: 'assets/15', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 14 },</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -688,7 +688,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:309, z:-269, id: 'p16', imageUrl: 'assets/16', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:309, z:-269, id: 'p16', imageUrl: 'assets/16', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 15 },</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -704,7 +704,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:275, z:-78, id: 'p17', imageUrl: 'assets/17', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:275, z:-78, id: 'p17', imageUrl: 'assets/17', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 16 },</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -720,7 +720,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:97, z:-228, id: 'p18', imageUrl: 'assets/18', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:97, z:-228, id: 'p18', imageUrl: 'assets/18', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 17 },</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -736,7 +736,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:107, z:-57, id: 'p19', imageUrl: 'assets/19', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:107, z:-57, id: 'p19', imageUrl: 'assets/19', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 18 },</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -752,7 +752,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:94, z:230, id: 'p20', imageUrl: 'assets/20', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:94, z:230, id: 'p20', imageUrl: 'assets/20', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 19 },</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -768,7 +768,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:70, z:418, id: 'p21', imageUrl: 'assets/21', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:70, z:418, id: 'p21', imageUrl: 'assets/21', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 20 },</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -784,7 +784,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:59, z:579, id: 'p22', imageUrl: 'assets/22', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:59, z:579, id: 'p22', imageUrl: 'assets/22', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 21 },</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -800,7 +800,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:51, z:845, id: 'p23', imageUrl: 'assets/23', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:51, z:845, id: 'p23', imageUrl: 'assets/23', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 22 },</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -816,7 +816,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:95, z:840, id: 'p24', imageUrl: 'assets/24', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:95, z:840, id: 'p24', imageUrl: 'assets/24', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 23 },</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -832,12 +832,11 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>{ x:75, z:772, id: 'p25', imageUrl: 'assets/25', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '' },</v>
+        <v>{ x:75, z:772, id: 'p25', imageUrl: 'assets/25', vaov: 180, vOffset: 0, maxpitch: 40, minpitch: -90, htmlContent: '', index: 24 },</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>